<commit_message>
risks analysis added to cli
</commit_message>
<xml_diff>
--- a/tests/resources/test_risk_master_1_2020.xlsx
+++ b/tests/resources/test_risk_master_1_2020.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="141">
   <si>
     <t xml:space="preserve">Project/Programme Name</t>
   </si>
@@ -421,7 +421,28 @@
     <t xml:space="preserve">DfT Group</t>
   </si>
   <si>
+    <t xml:space="preserve">Rail</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HSMRPG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AMIS</t>
+  </si>
+  <si>
     <t xml:space="preserve">IPDC approval point</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FBC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OBC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SOBC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pre-SOBC</t>
   </si>
 </sst>
 </file>
@@ -537,7 +558,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="76" zoomScaleNormal="76" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A83" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A95" activeCellId="0" sqref="A95"/>
+      <selection pane="bottomLeft" activeCell="F95" activeCellId="0" sqref="F95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1822,10 +1843,40 @@
       <c r="A94" s="1" t="s">
         <v>132</v>
       </c>
+      <c r="B94" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="C94" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="D94" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="E94" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="F94" s="1" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="1" t="s">
-        <v>133</v>
+        <v>136</v>
+      </c>
+      <c r="B95" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C95" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="D95" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="E95" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="F95" s="1" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>